<commit_message>
Updated to avoid request length and volume limits for tagging and reporting
</commit_message>
<xml_diff>
--- a/STAAS_Config.xlsx
+++ b/STAAS_Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\prosham\Src\STAAS-Reporting-Fusion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prosham/Library/CloudStorage/GoogleDrive-prosham@purestorage.com/My Drive/prosham/Src/STAAS-Reporting-Fusion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B677992-268C-4AE2-9DF9-0950DD91740F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B11A47F-D0F0-524E-BFF2-16BF0EC616C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1222" yWindow="11190" windowWidth="33841" windowHeight="10095" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="9260" windowWidth="33840" windowHeight="10100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fleet" sheetId="3" r:id="rId1"/>
@@ -21,31 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
-  <si>
-    <t>App1</t>
-  </si>
-  <si>
-    <t>App2</t>
-  </si>
-  <si>
-    <t>App3</t>
-  </si>
-  <si>
-    <t>App4</t>
-  </si>
-  <si>
-    <t>App5</t>
-  </si>
-  <si>
-    <t>App6</t>
-  </si>
-  <si>
-    <t>App7</t>
-  </si>
-  <si>
-    <t>App8</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>FUSION_SERVER</t>
   </si>
@@ -57,84 +33,6 @@
   </si>
   <si>
     <t>Telstra-STAAS</t>
-  </si>
-  <si>
-    <t>Application</t>
-  </si>
-  <si>
-    <t>App9</t>
-  </si>
-  <si>
-    <t>App10</t>
-  </si>
-  <si>
-    <t>App11</t>
-  </si>
-  <si>
-    <t>App12</t>
-  </si>
-  <si>
-    <t>App13</t>
-  </si>
-  <si>
-    <t>App14</t>
-  </si>
-  <si>
-    <t>App15</t>
-  </si>
-  <si>
-    <t>App16</t>
-  </si>
-  <si>
-    <t>App17</t>
-  </si>
-  <si>
-    <t>App18</t>
-  </si>
-  <si>
-    <t>App19</t>
-  </si>
-  <si>
-    <t>App20</t>
-  </si>
-  <si>
-    <t>App21</t>
-  </si>
-  <si>
-    <t>App22</t>
-  </si>
-  <si>
-    <t>App23</t>
-  </si>
-  <si>
-    <t>App24</t>
-  </si>
-  <si>
-    <t>App25</t>
-  </si>
-  <si>
-    <t>App26</t>
-  </si>
-  <si>
-    <t>App27</t>
-  </si>
-  <si>
-    <t>App28</t>
-  </si>
-  <si>
-    <t>App29</t>
-  </si>
-  <si>
-    <t>App30</t>
-  </si>
-  <si>
-    <t>App31</t>
-  </si>
-  <si>
-    <t>App32</t>
-  </si>
-  <si>
-    <t>IT</t>
   </si>
   <si>
     <t>Tag_By</t>
@@ -203,6 +101,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -444,200 +343,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C44270D-3563-0E45-A338-3DEA83E1D2E2}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -656,31 +390,31 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1">
         <v>1000</v>
@@ -688,12 +422,12 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1001</v>
@@ -701,12 +435,12 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>1002</v>
@@ -714,12 +448,12 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>1003</v>
@@ -727,12 +461,12 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1004</v>
@@ -740,12 +474,12 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1005</v>
@@ -753,19 +487,19 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>

</xml_diff>